<commit_message>
- HoaDonBaoHanh: remove colum {MaHoaDonGoc}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Temp_HoaDonBaoHanh.xlsx
+++ b/banhang24/Template/ExportExcel/Temp_HoaDonBaoHanh.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Thời gian:</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Trạng thái</t>
-  </si>
-  <si>
-    <t>Mã hóa đơn gốc</t>
   </si>
   <si>
     <t>DANH SÁCH HÓA ĐƠN BẢO HÀNH</t>
@@ -489,31 +486,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.5703125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="17" customWidth="1"/>
-    <col min="8" max="8" width="32.140625" style="17" customWidth="1"/>
-    <col min="9" max="9" width="29" style="17" customWidth="1"/>
-    <col min="10" max="11" width="24.140625" style="17" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" style="19" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="3" width="20.5703125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" style="17" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="29" style="17" customWidth="1"/>
+    <col min="9" max="10" width="24.140625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -526,10 +522,9 @@
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
       <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -540,465 +535,435 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" s="9" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" s="9" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>14</v>
+      <c r="B6" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="D6" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="E6" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="13"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K7" s="14"/>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K8" s="14"/>
+      <c r="L8" s="13"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="13"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K9" s="14"/>
+      <c r="L9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K10" s="14"/>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K11" s="14"/>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K12" s="14"/>
+      <c r="L12" s="13"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="13"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K13" s="14"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="13"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K14" s="14"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="13"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K15" s="14"/>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="13"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K16" s="14"/>
+      <c r="L16" s="13"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="13"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K17" s="14"/>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="13"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K18" s="14"/>
+      <c r="L18" s="13"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="13"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K19" s="14"/>
+      <c r="L19" s="13"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="13"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K20" s="14"/>
+      <c r="L20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="13"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="14"/>
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="13"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K22" s="14"/>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="13"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="14"/>
+      <c r="L23" s="13"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="13"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K24" s="14"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="13"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K25" s="14"/>
+      <c r="L25" s="13"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="13"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K26" s="14"/>
+      <c r="L26" s="13"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="13"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K27" s="14"/>
+      <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="13"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K28" s="14"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="13"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K29" s="14"/>
+      <c r="L29" s="13"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="13"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K30" s="14"/>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1007,13 +972,12 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="K32" s="15"/>
       <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>